<commit_message>
Upload project excluding Gaussian folder
</commit_message>
<xml_diff>
--- a/Project/Data:Analysis/Data.xlsx
+++ b/Project/Data:Analysis/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jh121/Library/Mobile Documents/com~apple~CloudDocs/Project/Data:Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FEEF23E-77DE-D244-BA3B-47CE5E4E3380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{260FBE9A-8C06-7E4D-B9C5-B9E85EDD3485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30860" windowHeight="16380" xr2:uid="{E2427F83-B15F-C447-AD0B-5A75AE5279B3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30860" windowHeight="16380" activeTab="5" xr2:uid="{E2427F83-B15F-C447-AD0B-5A75AE5279B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Base 1" sheetId="5" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="69">
   <si>
     <t>Molecule</t>
   </si>
@@ -249,6 +249,9 @@
   </si>
   <si>
     <t>ClosedR</t>
+  </si>
+  <si>
+    <t>ClosedRing</t>
   </si>
 </sst>
 </file>
@@ -1717,7 +1720,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B869D4D7-EA14-8F4B-A083-6A883E8B3107}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -3247,8 +3250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAE5031B-F0CE-104F-8605-A2754B2063CA}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3300,7 +3303,9 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="8"/>
+      <c r="A2" s="8" t="s">
+        <v>68</v>
+      </c>
       <c r="B2" s="8" t="s">
         <v>66</v>
       </c>
@@ -3345,7 +3350,9 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="8"/>
+      <c r="A3" s="8" t="s">
+        <v>68</v>
+      </c>
       <c r="B3" s="8" t="s">
         <v>67</v>
       </c>

</xml_diff>